<commit_message>
TAMID Alpha Newsletter V3
</commit_message>
<xml_diff>
--- a/portfolio_reports_1-31-23/alpha_regression.xlsx
+++ b/portfolio_reports_1-31-23/alpha_regression.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcu\Documents\University of Miami\Clubs\TAMID\Quant Group\Portfolio Newsletter\portfolio_reports_1-31-23\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42F21B4-B7CC-4A52-83D6-6B4BC6ED13C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="0" windowWidth="28785" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>TAMID ~ SPY</t>
   </si>
@@ -36,15 +30,12 @@
   <si>
     <t>Beta T-Stat</t>
   </si>
-  <si>
-    <t>Alpha Regression</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,15 +51,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -78,7 +60,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,19 +69,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
@@ -112,86 +83,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -199,14 +98,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -253,7 +144,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,27 +176,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -337,24 +210,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -530,57 +385,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
-        <v>0.621</v>
+      <c r="B2">
+        <v>0.156</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
-        <v>1.98</v>
+      <c r="B3">
+        <v>1.487</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
-        <v>1.2569999999999999</v>
+      <c r="B4">
+        <v>1.299</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <v>14.917999999999999</v>
+      <c r="B5">
+        <v>43.243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>